<commit_message>
updated code: added question number updated parameters file
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YuChen\PycharmProjects\GoogleAlerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6C2364-B830-4D27-AAAC-8D616D3FE7DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF8C4B9-BA08-41D3-B49D-72C28ECC04B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10785" yWindow="3000" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>BoardReader</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Keyword</t>
   </si>
   <si>
-    <t>covid19</t>
-  </si>
-  <si>
     <t>GoogleAlerts</t>
   </si>
   <si>
@@ -46,6 +43,21 @@
   </si>
   <si>
     <t>Number of articles:</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Question 1</t>
+  </si>
+  <si>
+    <t>Question 2</t>
+  </si>
+  <si>
+    <t>Paragraph</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
@@ -363,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,42 +387,55 @@
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated code: added twitter scrapper
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YuChen\PycharmProjects\GoogleAlerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF8C4B9-BA08-41D3-B49D-72C28ECC04B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240569F0-9CFB-484A-BC0B-8B529B8096B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="2190" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>BoardReader</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Number of articles:</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>Question 1</t>
   </si>
   <si>
@@ -57,7 +54,10 @@
     <t>Paragraph</t>
   </si>
   <si>
-    <t>Source</t>
+    <t>#istandwithraeesahkhan</t>
+  </si>
+  <si>
+    <t>#istandwithraeesahkhan site: twitter.com</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,10 +398,10 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -409,19 +409,16 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -429,13 +426,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated code: updated Parameters.xlsx fixed concetatnation
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YuChen\PycharmProjects\GoogleAlerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240569F0-9CFB-484A-BC0B-8B529B8096B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759F3D71-3529-412F-9B87-34A71DB86154}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="2190" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="120" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,47 +25,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>BoardReader</t>
-  </si>
-  <si>
-    <t>Number of articles</t>
-  </si>
-  <si>
-    <t>Keyword</t>
-  </si>
-  <si>
-    <t>GoogleAlerts</t>
-  </si>
-  <si>
-    <t>Keyword:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Number of articles:</t>
   </si>
   <si>
-    <t>Question 1</t>
-  </si>
-  <si>
-    <t>Question 2</t>
-  </si>
-  <si>
-    <t>Paragraph</t>
-  </si>
-  <si>
-    <t>#istandwithraeesahkhan</t>
-  </si>
-  <si>
-    <t>#istandwithraeesahkhan site: twitter.com</t>
+    <t>GoogleAlerts Keyword:</t>
+  </si>
+  <si>
+    <t>BoardReaderKeyword:</t>
+  </si>
+  <si>
+    <t>For Google Alerts</t>
+  </si>
+  <si>
+    <t>For BoardReader</t>
+  </si>
+  <si>
+    <t>For Topic Modelling</t>
+  </si>
+  <si>
+    <t>Number of Questions:</t>
+  </si>
+  <si>
+    <t>Question 1:</t>
+  </si>
+  <si>
+    <t>Question 2:</t>
+  </si>
+  <si>
+    <t>Question 3:</t>
+  </si>
+  <si>
+    <t>Question 4:</t>
+  </si>
+  <si>
+    <t>Name of Excel File</t>
+  </si>
+  <si>
+    <t>For Twitter</t>
+  </si>
+  <si>
+    <t>Twitter Keyword:</t>
+  </si>
+  <si>
+    <t>Name of Sheet:</t>
+  </si>
+  <si>
+    <t>#istandwithraeesah</t>
+  </si>
+  <si>
+    <t>max = 75</t>
+  </si>
+  <si>
+    <t>max = 1000</t>
+  </si>
+  <si>
+    <t>no max</t>
+  </si>
+  <si>
+    <t>14-07-20 1454</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Number of Topics:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,8 +134,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,67 +418,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated code: updated code
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YuChen\PycharmProjects\GoogleAlerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759F3D71-3529-412F-9B87-34A71DB86154}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F0538C-B566-4C30-AC1F-BEA496C26F09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="120" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Number of articles:</t>
   </si>
@@ -84,13 +84,25 @@
     <t>no max</t>
   </si>
   <si>
-    <t>14-07-20 1454</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>Number of Topics:</t>
+  </si>
+  <si>
+    <t>FY2019 MOC quali data</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>C04</t>
   </si>
 </sst>
 </file>
@@ -421,7 +433,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +516,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -512,15 +524,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -528,7 +540,7 @@
         <v>6</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,22 +548,31 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: added more comments
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YuChen\PycharmProjects\GoogleAlerts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yc_19\OneDrive\Documents\GitHub\GoogleAlerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F0538C-B566-4C30-AC1F-BEA496C26F09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4433EEEE-A01E-4EC0-90C4-B4C052D56EE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Number of articles:</t>
   </si>
@@ -45,21 +45,6 @@
     <t>For Topic Modelling</t>
   </si>
   <si>
-    <t>Number of Questions:</t>
-  </si>
-  <si>
-    <t>Question 1:</t>
-  </si>
-  <si>
-    <t>Question 2:</t>
-  </si>
-  <si>
-    <t>Question 3:</t>
-  </si>
-  <si>
-    <t>Question 4:</t>
-  </si>
-  <si>
     <t>Name of Excel File</t>
   </si>
   <si>
@@ -72,9 +57,6 @@
     <t>Name of Sheet:</t>
   </si>
   <si>
-    <t>#istandwithraeesah</t>
-  </si>
-  <si>
     <t>max = 75</t>
   </si>
   <si>
@@ -87,22 +69,19 @@
     <t>Number of Topics:</t>
   </si>
   <si>
-    <t>FY2019 MOC quali data</t>
-  </si>
-  <si>
-    <t>Master</t>
-  </si>
-  <si>
-    <t>C01</t>
-  </si>
-  <si>
-    <t>C02</t>
-  </si>
-  <si>
-    <t>C03</t>
-  </si>
-  <si>
-    <t>C04</t>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>follows keyword in B2</t>
+  </si>
+  <si>
+    <t>covid19</t>
+  </si>
+  <si>
+    <t>#markinourhearts</t>
+  </si>
+  <si>
+    <t>03-08-20 1432</t>
   </si>
 </sst>
 </file>
@@ -430,153 +409,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
       <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated code: Mostly done
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yc_19\OneDrive\Documents\GitHub\GoogleAlerts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YuChen\PycharmProjects\GoogleAlerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4433EEEE-A01E-4EC0-90C4-B4C052D56EE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDA9E7C-F60A-4B9E-A112-68D62541AE49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4635" yWindow="3150" windowWidth="18795" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Number of articles:</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>03-08-20 1432</t>
+  </si>
+  <si>
+    <t>#istandwithraeesah</t>
   </si>
 </sst>
 </file>
@@ -411,21 +414,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -433,7 +436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -441,7 +444,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -452,12 +455,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -465,7 +468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -476,20 +479,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -500,12 +503,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -513,7 +516,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -521,7 +524,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>